<commit_message>
update tests & testLog File
</commit_message>
<xml_diff>
--- a/variables.xlsx
+++ b/variables.xlsx
@@ -8,24 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yarden\git\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F06CF8-EADA-496F-A01C-1A85A5C8F791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE5D65D-97C2-4A75-88E6-5D2BF8A1B5E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29760" yWindow="960" windowWidth="21600" windowHeight="11430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>userName</t>
   </si>
@@ -55,6 +65,48 @@
   </si>
   <si>
     <t>Git</t>
+  </si>
+  <si>
+    <t>regFName</t>
+  </si>
+  <si>
+    <t>regLName</t>
+  </si>
+  <si>
+    <t>Jordi</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>regUserName</t>
+  </si>
+  <si>
+    <t>JordiD</t>
+  </si>
+  <si>
+    <t>regPassword</t>
+  </si>
+  <si>
+    <t>RamiMaHakesher1#</t>
+  </si>
+  <si>
+    <t>regWrongPassword</t>
+  </si>
+  <si>
+    <t>Ya111111</t>
+  </si>
+  <si>
+    <t>regWrongPasswordMSG</t>
+  </si>
+  <si>
+    <t>Passwords must have at least one non alphanumeric character, one digit ('0'-'9'), one uppercase ('A'-'Z'), one lowercase ('a'-'z'), one special character and Password must be eight characters or longer.</t>
+  </si>
+  <si>
+    <t>regCaptchaMSG</t>
+  </si>
+  <si>
+    <t>Please verify reCaptcha to register!</t>
   </si>
 </sst>
 </file>
@@ -96,7 +148,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -372,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -420,7 +483,66 @@
         <v>9</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="A8:B8">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>